<commit_message>
fix row addition to resultSimulation and fix rocketDict params
</commit_message>
<xml_diff>
--- a/simulationResults.xlsx
+++ b/simulationResults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alec\Desktop\Code\GTXR\AutoRASAero\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alecd\Desktop\Code\GTXR\AutoRASAero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5F51A6A-FA27-4647-A958-4DC5683AA894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B7D53EA-0E32-42A2-877A-B06FCEBCAD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{55ADB120-79C2-45CC-BC9E-CA6DDA91E05A}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8964" xr2:uid="{34B33473-12D8-44A7-90E5-7FE250FC3705}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
   <si>
     <t>Booster Start Stability</t>
   </si>
@@ -56,16 +56,37 @@
   </si>
   <si>
     <t>Apogee</t>
+  </si>
+  <si>
+    <t>test 1</t>
+  </si>
+  <si>
+    <t>test 2</t>
+  </si>
+  <si>
+    <t>test 3</t>
+  </si>
+  <si>
+    <t>test 4</t>
+  </si>
+  <si>
+    <t>test 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -406,24 +427,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DDF8F5-A5DC-402E-A845-E49B168AD70D}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B31118F-1F4B-4DE6-BC13-F45586BA002D}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +459,123 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>